<commit_message>
create join team api calls added
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>S.No</t>
   </si>
@@ -42,9 +42,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>api/GetTeamInfo/{SecretNumber}</t>
-  </si>
-  <si>
     <t>api/jointeam? SecretNumber=secretnumber &amp; MemberName=memebrename</t>
   </si>
   <si>
@@ -58,13 +55,112 @@
   </si>
   <si>
     <t>TEAMS</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>api/CreateFile</t>
+  </si>
+  <si>
+    <t>{
+    "Path":"~/Projects/team3",
+    "FileName":"scripts.js"
+}</t>
+  </si>
+  <si>
+    <t>api/CreateFolder</t>
+  </si>
+  <si>
+    <t>{
+    "Path":"~/Projects/team3",
+    "FolderName":"scripts"
+}</t>
+  </si>
+  <si>
+    <t>api/updatefile</t>
+  </si>
+  <si>
+    <t>{
+    "Path":"~/Projects/team3/index.html",
+    "Content":"&lt;h1&gt;Index.html&lt;/h1&gt;&lt;p&gt;this is body&lt;/p&gt;"
+}</t>
+  </si>
+  <si>
+    <t>api/GetFileContent</t>
+  </si>
+  <si>
+    <t>{
+    "Path":"~/Projects/team1/index.html"
+}</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>{
+    "CurrentMember": {
+        "Id": 19,
+        "Name": "asdasd",
+        "TeamId": 25
+    },
+    "Team": {
+        "Id": 25,
+        "TeamName": "asdasd",
+        "SecretNumber": "dZAWNvxE",
+        "FolderPath": "~/Projects/asdasd",
+        "CreatedOn": "2022-02-21T13:53:29.923",
+        "ClosedOn": "0001-01-01T00:00:00"
+    },
+    "Members": []
+}</t>
+  </si>
+  <si>
+    <t>{
+    "CurrentMember": {
+        "Id": 22,
+        "Name": "irfann",
+        "TeamId": 25
+    },
+    "Team": {
+        "Id": 25,
+        "TeamName": "asdasd",
+        "SecretNumber": "dZAWNvxE",
+        "FolderPath": "~/Projects/asdasd",
+        "CreatedOn": "2022-02-21T13:53:29.923",
+        "ClosedOn": "0001-01-01T00:00:00"
+    },
+    "Members": [
+        {
+            "Id": 19,
+            "Name": "asdasd",
+            "TeamId": 25
+        },
+        {
+            "Id": 20,
+            "Name": "irfan",
+            "TeamId": 25
+        },
+        {
+            "Id": 21,
+            "Name": "irfan",
+            "TeamId": 25
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>api/GetTeamInfo/{SecretNumber}/{CurrentMembername}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,14 +170,34 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +210,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,18 +229,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Accent5" xfId="3" builtinId="45"/>
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,228 +566,388 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="409.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>14</v>
-      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
left panel routing init | local storage
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>S.No</t>
   </si>
@@ -188,6 +188,20 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>[
+    "index.html",
+    "scripts.js"
+]</t>
+  </si>
+  <si>
+    <t>{
+    "Path":"~/Projects/team1"
+}</t>
+  </si>
+  <si>
+    <t>api/GetDirectoryStructure</t>
   </si>
 </sst>
 </file>
@@ -314,14 +328,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -609,7 +623,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +637,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -681,19 +695,19 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -757,14 +771,22 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -821,13 +843,13 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">

</xml_diff>